<commit_message>
Fixed bugs. Changes in the locking mechanism. Changes in visual style
</commit_message>
<xml_diff>
--- a/Products.xlsx
+++ b/Products.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\londelord\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\londelord\Documents\TestTasks\Intravision\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A59FF4F-20FC-41A3-90B9-2276F712291E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A50B13A-1381-443A-BC12-AAFEBB802075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -70,16 +70,48 @@
   </si>
   <si>
     <t>Schweppes 1l</t>
+  </si>
+  <si>
+    <t>ImageUrl</t>
+  </si>
+  <si>
+    <t>https://bevmo.com/cdn/shop/files/fb765f7c-0dcb-406e-9e05-a2d274c7209d.png?v=1731685327</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/3/36/Dr_Pepper_0%2C33l_Dose_Classic.png</t>
+  </si>
+  <si>
+    <t>https://www.pngplay.com/wp-content/uploads/15/Sprite-Can-PNG-Background.png</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRJ6OBfTWkIslL48co4uwgiz1QqfWeIrU1nKg&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTGeaoa9E51bvbXWFr51XrdH3JOKr3YeUzC5w&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTqQmTKrzJPVC6y210ra1eRbiYfDkp2HtQddA&amp;s</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSIa8j5iWu2Hh4RQIZYORO9mzb-L7HNf9QUMQ&amp;s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,13 +134,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -387,19 +422,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="98.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,8 +448,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -426,8 +465,11 @@
       <c r="D2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -440,8 +482,11 @@
       <c r="D3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -454,8 +499,11 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -468,8 +516,11 @@
       <c r="D5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -482,8 +533,11 @@
       <c r="D6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -496,8 +550,11 @@
       <c r="D7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -510,8 +567,11 @@
       <c r="D8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -524,8 +584,11 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -538,8 +601,11 @@
       <c r="D10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -552,8 +618,11 @@
       <c r="D11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -565,6 +634,9 @@
       </c>
       <c r="D12">
         <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>